<commit_message>
chore: Students Update According to #55
</commit_message>
<xml_diff>
--- a/public/excel_import_template/students_import.xlsx
+++ b/public/excel_import_template/students_import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
   <si>
     <t xml:space="preserve">Nama</t>
   </si>
@@ -40,7 +40,10 @@
     <t xml:space="preserve">Agama</t>
   </si>
   <si>
-    <t xml:space="preserve">No Telepon</t>
+    <t xml:space="preserve">Nomor Telepon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nomor Kartu Keluarga</t>
   </si>
   <si>
     <t xml:space="preserve">NIK</t>
@@ -55,46 +58,37 @@
     <t xml:space="preserve">Nama Ayah</t>
   </si>
   <si>
-    <t xml:space="preserve">Tanggal Lahir Ayah</t>
+    <t xml:space="preserve">Alamat Ayah</t>
   </si>
   <si>
     <t xml:space="preserve">Pekerjaan Ayah</t>
   </si>
   <si>
-    <t xml:space="preserve">Edukasi Terakhir Ayah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pendapatan Ayah</t>
+    <t xml:space="preserve">Nomor Telepon Ayah</t>
   </si>
   <si>
     <t xml:space="preserve">Nama Ibu</t>
   </si>
   <si>
-    <t xml:space="preserve">Tanggal Lahir Ibu</t>
+    <t xml:space="preserve">Alamat Ibu</t>
   </si>
   <si>
     <t xml:space="preserve">Pekerjaan Ibu</t>
   </si>
   <si>
-    <t xml:space="preserve">Edukasi Terakhir Ibu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pendapatan Ibu</t>
+    <t xml:space="preserve">Nomor Telepon Ibu</t>
   </si>
   <si>
     <t xml:space="preserve">Nama Wali</t>
   </si>
   <si>
-    <t xml:space="preserve">Tanggal Lahir Wali</t>
+    <t xml:space="preserve">Alamat Wali</t>
   </si>
   <si>
     <t xml:space="preserve">Pekerjaan Wali</t>
   </si>
   <si>
-    <t xml:space="preserve">Edukasi Terakhir Wali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pendapatan Wali</t>
+    <t xml:space="preserve">Nomor Telepon Wali</t>
   </si>
   <si>
     <t xml:space="preserve">Lukita Jamil Siregar S.IP</t>
@@ -112,15 +106,24 @@
     <t xml:space="preserve">Kristen</t>
   </si>
   <si>
+    <t xml:space="preserve">081295728943</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3487892850195783</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5829489125912859</t>
+  </si>
+  <si>
     <t xml:space="preserve">Harjasa Parman Saptono</t>
   </si>
   <si>
+    <t xml:space="preserve">Jr. Dipenogoro No. 345, Bandung 42213, Banten</t>
+  </si>
+  <si>
     <t xml:space="preserve">Penyiar Radio</t>
   </si>
   <si>
-    <t xml:space="preserve">SMA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ilsa Melani</t>
   </si>
   <si>
@@ -130,6 +133,9 @@
     <t xml:space="preserve">Rachel Wastuti</t>
   </si>
   <si>
+    <t xml:space="preserve">Psr. Halim No. 905, Sawahlunto 14347, DIY</t>
+  </si>
+  <si>
     <t xml:space="preserve">Paraji</t>
   </si>
   <si>
@@ -145,15 +151,30 @@
     <t xml:space="preserve">Ds. Muwardi No. 392, Padangsidempuan 94704, Sulteng</t>
   </si>
   <si>
+    <t xml:space="preserve">085812429402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3189387567802982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1938297488273948</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bakiman Galiono Iswahyudi</t>
   </si>
   <si>
+    <t xml:space="preserve">Gg. Suryo No. 182, Payakumbuh 97153, Riau</t>
+  </si>
+  <si>
     <t xml:space="preserve">Perancang Busana</t>
   </si>
   <si>
     <t xml:space="preserve">Queen Suartini</t>
   </si>
   <si>
+    <t xml:space="preserve">Kpg. Gading No. 791, Lhokseumawe 74003, Bengkulu</t>
+  </si>
+  <si>
     <t xml:space="preserve">Konstruksi</t>
   </si>
   <si>
@@ -166,9 +187,21 @@
     <t xml:space="preserve">Jr. Asia Afrika No. 790, Sungai Penuh 42835, Kalsel</t>
   </si>
   <si>
+    <t xml:space="preserve">089285782935</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‘3289587148917348</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6278498127384912</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ikhsan Pangestu</t>
   </si>
   <si>
+    <t xml:space="preserve">Ds. Supomo No. 961, Palembang 80017, Bali</t>
+  </si>
+  <si>
     <t xml:space="preserve">Transportasi</t>
   </si>
   <si>
@@ -178,25 +211,23 @@
     <t xml:space="preserve">Karyawan Swasta</t>
   </si>
   <si>
-    <t xml:space="preserve">SMP</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yuliana Usyi Halimah</t>
   </si>
   <si>
+    <t xml:space="preserve">Ds. Tubagus Ismail No. 951, Magelang 63012, Kalbar</t>
+  </si>
+  <si>
     <t xml:space="preserve">Penata Busana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -285,7 +316,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -298,7 +329,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -379,16 +414,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V3" activeCellId="0" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="1" style="1" width="30.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="26" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="1" style="1" width="30.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="24" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -413,7 +448,7 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -460,229 +495,208 @@
       </c>
       <c r="W1" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="4" t="n">
+        <v>37948</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="3" t="n">
-        <v>37948</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="1" t="n">
-        <v>819204502</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>212957885</v>
-      </c>
-      <c r="I2" s="1" t="n">
+      <c r="I2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="1" t="n">
         <v>715311312</v>
       </c>
-      <c r="J2" s="1" t="n">
+      <c r="K2" s="1" t="n">
         <v>117047387</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="3" t="n">
-        <v>32277</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="M2" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>706946036</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="1" t="n">
-        <v>8573290</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" s="3" t="n">
-        <v>32899</v>
-      </c>
       <c r="R2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" s="1" t="n">
-        <v>7000000</v>
-      </c>
-      <c r="U2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="V2" s="3" t="n">
-        <v>32071</v>
-      </c>
-      <c r="W2" s="1" t="s">
+      <c r="S2" s="1" t="n">
+        <v>611875383</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y2" s="1" t="n">
-        <v>8000000</v>
+      <c r="U2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" s="1" t="n">
+        <v>987958880</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="E3" s="4" t="n">
         <v>37836</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>102808431</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>852584950</v>
-      </c>
-      <c r="I3" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="1" t="n">
         <v>533685358</v>
       </c>
-      <c r="J3" s="1" t="n">
+      <c r="K3" s="1" t="n">
         <v>983472148</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" s="3" t="n">
-        <v>32542</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>42</v>
+      <c r="L3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="O3" s="1" t="n">
-        <v>5649510</v>
+        <v>806298070</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q3" s="3" t="n">
-        <v>32489</v>
+        <v>49</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="T3" s="1" t="n">
-        <v>745418</v>
-      </c>
-      <c r="V3" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>133124861</v>
+      </c>
+      <c r="U3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>38103</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="3" t="n">
-        <v>38103</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>348211020</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>369736255</v>
-      </c>
-      <c r="I4" s="1" t="n">
+      <c r="G4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="1" t="n">
         <v>130112285</v>
       </c>
-      <c r="J4" s="1" t="n">
+      <c r="K4" s="1" t="n">
         <v>396580957</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L4" s="3" t="n">
-        <v>30457</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>49</v>
+      <c r="L4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="O4" s="1" t="n">
-        <v>3636915</v>
+        <v>491574179</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q4" s="3" t="n">
-        <v>33650</v>
+        <v>61</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T4" s="1" t="n">
-        <v>8434437</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="V4" s="3" t="n">
-        <v>30770</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y4" s="1" t="n">
-        <v>1791464</v>
+        <v>62</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>206641846</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W4" s="1" t="n">
+        <v>482675675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>